<commit_message>
fixed typo in question name
</commit_message>
<xml_diff>
--- a/hamed/fixtures/scan-certificat.xlsx
+++ b/hamed/fixtures/scan-certificat.xlsx
@@ -138,13 +138,13 @@
     <t>pulldata("targets", "age", "ident", ${ident})</t>
   </si>
   <si>
-    <t>certifcat-indigence</t>
-  </si>
-  <si>
     <t>certificat-residence</t>
   </si>
   <si>
     <t>Photo du certificat de résidence</t>
+  </si>
+  <si>
+    <t>certificat-indigence</t>
   </si>
 </sst>
 </file>
@@ -490,7 +490,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,7 +643,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
@@ -663,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>

</xml_diff>